<commit_message>
Hello and color added
</commit_message>
<xml_diff>
--- a/Testing1.xlsx
+++ b/Testing1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Fichiers_Excel_Adam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A8602CD-AAB0-4546-9B48-C442854413C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6412346B-6AE3-4527-969E-E7A6422F2400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{4545AC7C-3C80-4303-8765-C5315DD7A457}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4545AC7C-3C80-4303-8765-C5315DD7A457}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>Hello!</t>
   </si>
 </sst>
 </file>
@@ -52,12 +55,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,15 +398,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA304BF-91B1-42EC-B416-801C590A4005}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -416,6 +426,11 @@
       </c>
       <c r="C2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>